<commit_message>
Updated 'Criterios por estado' table with total values
</commit_message>
<xml_diff>
--- a/criterios_por_estado.xlsx
+++ b/criterios_por_estado.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1914,6 +1914,58 @@
         <v>100</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>36.22</v>
+      </c>
+      <c r="D29" t="n">
+        <v>10.41</v>
+      </c>
+      <c r="E29" t="n">
+        <v>81.89</v>
+      </c>
+      <c r="F29" t="n">
+        <v>44.45</v>
+      </c>
+      <c r="G29" t="n">
+        <v>99.45</v>
+      </c>
+      <c r="H29" t="n">
+        <v>86.78</v>
+      </c>
+      <c r="I29" t="n">
+        <v>74.67</v>
+      </c>
+      <c r="J29" t="n">
+        <v>40.23</v>
+      </c>
+      <c r="K29" t="n">
+        <v>10.82</v>
+      </c>
+      <c r="L29" t="n">
+        <v>10.17</v>
+      </c>
+      <c r="M29" t="n">
+        <v>51.31</v>
+      </c>
+      <c r="N29" t="n">
+        <v>8.279999999999999</v>
+      </c>
+      <c r="O29" t="n">
+        <v>70.86</v>
+      </c>
+      <c r="P29" t="n">
+        <v>99.38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>